<commit_message>
fix: Rerun CODEX metadata reharmonization procedure
</commit_message>
<xml_diff>
--- a/metadata/codex/todo/Stanford TMC (CODEX).xlsx
+++ b/metadata/codex/todo/Stanford TMC (CODEX).xlsx
@@ -13,7 +13,7 @@
     <sheet name="Invalid Input Pattern" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Missing Required Value'!$A$1:$D$206</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Invalid Input Pattern'!$A$1:$F$68</definedName>
   </definedNames>
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,11 +436,6 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>In-House</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>hour</t>
         </is>
       </c>
@@ -453,11 +448,6 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Leica Biosystems</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>month</t>
         </is>
       </c>
@@ -470,11 +460,6 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Not applicable</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>year</t>
         </is>
       </c>
@@ -487,11 +472,6 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Thermo Fisher Scientific</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>day</t>
         </is>
       </c>
@@ -504,11 +484,6 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Roche Diagnostics</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>minute</t>
         </is>
       </c>
@@ -516,109 +491,96 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NanoZoomer S360</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>HTX Technologies</t>
+          <t>Custom</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NanoZoomer S60</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>10x Genomics</t>
+          <t>NanoZoomer S360</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Chromium X</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Hamamatsu</t>
+          <t>NanoZoomer S60</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AutoStainer XL</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SunChrom</t>
+          <t>Chromium X</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Visium CytAssist</t>
+          <t>AutoStainer XL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SunCollect Sprayer</t>
+          <t>Visium CytAssist</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M3+ Sprayer</t>
+          <t>SunCollect Sprayer</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Discovery Ultra</t>
+          <t>M3+ Sprayer</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ST5020 Multistainer</t>
+          <t>Discovery Ultra</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chromium iX</t>
+          <t>ST5020 Multistainer</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chromium Connect</t>
+          <t>Chromium iX</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>M5 Sprayer</t>
+          <t>Chromium Connect</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
+        <is>
+          <t>M5 Sprayer</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>TM-Sprayer</t>
         </is>
@@ -635,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,30 +658,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HBM235.VKNJ.237</t>
+          <t>HBM238.GTNW.259</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM235.VKNJ.237</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM238.GTNW.259</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HBM238.GTNW.259</t>
+          <t>HBM242.LSCK.393</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -735,37 +697,37 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM238.GTNW.259</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM242.LSCK.393</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HBM238.GTNW.259</t>
+          <t>HBM284.SBPR.357</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM238.GTNW.259</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM284.SBPR.357</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HBM242.LSCK.393</t>
+          <t>HBM285.VFDT.966</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -781,37 +743,37 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM242.LSCK.393</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM285.VFDT.966</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HBM242.LSCK.393</t>
+          <t>HBM288.BBKK.828</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM242.LSCK.393</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM288.BBKK.828</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HBM284.SBPR.357</t>
+          <t>HBM295.SWJJ.888</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -827,37 +789,37 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM284.SBPR.357</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM295.SWJJ.888</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HBM284.SBPR.357</t>
+          <t>HBM297.MZZX.824</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM284.SBPR.357</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM297.MZZX.824</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HBM285.VFDT.966</t>
+          <t>HBM334.QWFV.953</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -873,37 +835,37 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM285.VFDT.966</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM334.QWFV.953</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HBM285.VFDT.966</t>
+          <t>HBM353.NZVQ.793</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM285.VFDT.966</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM353.NZVQ.793</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HBM288.BBKK.828</t>
+          <t>HBM363.CKHC.928</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -919,37 +881,37 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM288.BBKK.828</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM363.CKHC.928</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HBM288.BBKK.828</t>
+          <t>HBM363.LLBL.252</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM288.BBKK.828</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM363.LLBL.252</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HBM295.SWJJ.888</t>
+          <t>HBM394.VSKR.883</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -965,37 +927,37 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM295.SWJJ.888</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM394.VSKR.883</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HBM295.SWJJ.888</t>
+          <t>HBM395.NQKF.566</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM295.SWJJ.888</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM395.NQKF.566</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HBM297.MZZX.824</t>
+          <t>HBM424.STVV.842</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1005,43 +967,43 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM297.MZZX.824</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM424.STVV.842</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HBM297.MZZX.824</t>
+          <t>HBM429.LLRT.546</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM297.MZZX.824</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM429.LLRT.546</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HBM334.QWFV.953</t>
+          <t>HBM433.MQRQ.278</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1057,37 +1019,37 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM334.QWFV.953</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM433.MQRQ.278</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>HBM334.QWFV.953</t>
+          <t>HBM438.JXJW.249</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM334.QWFV.953</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM438.JXJW.249</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HBM353.NZVQ.793</t>
+          <t>HBM439.WJDV.974</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1103,37 +1065,37 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM353.NZVQ.793</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM439.WJDV.974</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HBM353.NZVQ.793</t>
+          <t>HBM443.LGZK.435</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM353.NZVQ.793</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM443.LGZK.435</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>HBM363.CKHC.928</t>
+          <t>HBM447.MNKW.592</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1149,37 +1111,37 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM363.CKHC.928</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM447.MNKW.592</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>HBM363.CKHC.928</t>
+          <t>HBM462.JKCN.863</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM363.CKHC.928</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM462.JKCN.863</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HBM363.LLBL.252</t>
+          <t>HBM465.ZNVW.226</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1195,37 +1157,37 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM363.LLBL.252</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM465.ZNVW.226</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>HBM363.LLBL.252</t>
+          <t>HBM466.XSKL.867</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM363.LLBL.252</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM466.XSKL.867</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HBM394.VSKR.883</t>
+          <t>HBM473.QGDG.848</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1241,37 +1203,37 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM394.VSKR.883</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM473.QGDG.848</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HBM394.VSKR.883</t>
+          <t>HBM488.CNNZ.544</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM394.VSKR.883</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM488.CNNZ.544</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HBM395.NQKF.566</t>
+          <t>HBM535.QNTP.246</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1287,37 +1249,37 @@
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM395.NQKF.566</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM535.QNTP.246</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>HBM395.NQKF.566</t>
+          <t>HBM565.LSMX.645</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM395.NQKF.566</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM565.LSMX.645</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HBM424.STVV.842</t>
+          <t>HBM569.NBHZ.832</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1327,43 +1289,43 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CODEX Instrument</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM424.STVV.842</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM569.NBHZ.832</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HBM424.STVV.842</t>
+          <t>HBM573.SWGH.988</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM424.STVV.842</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM573.SWGH.988</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>HBM429.LLRT.546</t>
+          <t>HBM573.TTLG.748</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1379,37 +1341,37 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM429.LLRT.546</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM573.TTLG.748</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>HBM429.LLRT.546</t>
+          <t>HBM575.THQM.284</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM429.LLRT.546</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM575.THQM.284</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>HBM433.MQRQ.278</t>
+          <t>HBM622.STKS.394</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1425,37 +1387,37 @@
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM433.MQRQ.278</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM622.STKS.394</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>HBM433.MQRQ.278</t>
+          <t>HBM626.VJMB.795</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM433.MQRQ.278</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM626.VJMB.795</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>HBM438.JXJW.249</t>
+          <t>HBM627.KDHD.293</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1471,37 +1433,37 @@
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM438.JXJW.249</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM627.KDHD.293</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HBM438.JXJW.249</t>
+          <t>HBM666.NDQZ.365</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM438.JXJW.249</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM666.NDQZ.365</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>HBM439.WJDV.974</t>
+          <t>HBM666.RBCG.529</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1517,37 +1479,37 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM439.WJDV.974</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM666.RBCG.529</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>HBM439.WJDV.974</t>
+          <t>HBM676.QVGZ.455</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM439.WJDV.974</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM676.QVGZ.455</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>HBM443.LGZK.435</t>
+          <t>HBM679.NNNK.283</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1557,43 +1519,43 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CODEX Instrument</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM443.LGZK.435</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM679.NNNK.283</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>HBM443.LGZK.435</t>
+          <t>HBM683.NRPR.962</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM443.LGZK.435</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM683.NRPR.962</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>HBM447.MNKW.592</t>
+          <t>HBM687.SJLD.889</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1603,43 +1565,43 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM447.MNKW.592</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM687.SJLD.889</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>HBM447.MNKW.592</t>
+          <t>HBM727.DMKG.675</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM447.MNKW.592</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM727.DMKG.675</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>HBM462.JKCN.863</t>
+          <t>HBM729.XTBN.693</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1649,43 +1611,43 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM462.JKCN.863</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM729.XTBN.693</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>HBM462.JKCN.863</t>
+          <t>HBM734.XBSR.357</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM462.JKCN.863</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM734.XBSR.357</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>HBM465.ZNVW.226</t>
+          <t>HBM739.HCWP.359</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1695,43 +1657,43 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM465.ZNVW.226</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM739.HCWP.359</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>HBM465.ZNVW.226</t>
+          <t>HBM742.NHHQ.357</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM465.ZNVW.226</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM742.NHHQ.357</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>HBM466.XSKL.867</t>
+          <t>HBM749.SMWP.555</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1747,37 +1709,37 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM466.XSKL.867</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM749.SMWP.555</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>HBM466.XSKL.867</t>
+          <t>HBM772.TKCN.287</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM466.XSKL.867</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM772.TKCN.287</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>HBM473.QGDG.848</t>
+          <t>HBM785.FJVT.469</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1793,37 +1755,37 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM473.QGDG.848</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM785.FJVT.469</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>HBM473.QGDG.848</t>
+          <t>HBM792.FFJT.499</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM473.QGDG.848</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM792.FFJT.499</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>HBM488.CNNZ.544</t>
+          <t>HBM823.RJNG.364</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1839,37 +1801,37 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM488.CNNZ.544</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM823.RJNG.364</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>HBM488.CNNZ.544</t>
+          <t>HBM824.XGWZ.857</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM488.CNNZ.544</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM824.XGWZ.857</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>HBM535.QNTP.246</t>
+          <t>HBM827.SJBP.777</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1885,37 +1847,37 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM535.QNTP.246</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM827.SJBP.777</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HBM535.QNTP.246</t>
+          <t>HBM832.ZSQJ.442</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM535.QNTP.246</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM832.ZSQJ.442</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>HBM565.LSMX.645</t>
+          <t>HBM845.VMSZ.536</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1931,37 +1893,37 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM565.LSMX.645</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM845.VMSZ.536</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>HBM565.LSMX.645</t>
+          <t>HBM852.NKST.623</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM565.LSMX.645</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM852.NKST.623</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HBM569.NBHZ.832</t>
+          <t>HBM865.VDXC.862</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1977,37 +1939,37 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM569.NBHZ.832</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM865.VDXC.862</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>HBM569.NBHZ.832</t>
+          <t>HBM893.MCGS.487</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM569.NBHZ.832</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM893.MCGS.487</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>HBM573.SWGH.988</t>
+          <t>HBM899.KTQM.246</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2023,37 +1985,37 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM573.SWGH.988</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM899.KTQM.246</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>HBM573.SWGH.988</t>
+          <t>HBM934.KLGL.584</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM573.SWGH.988</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM934.KLGL.584</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>HBM573.TTLG.748</t>
+          <t>HBM938.KMNW.825</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2069,37 +2031,37 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM573.TTLG.748</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM938.KMNW.825</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>HBM573.TTLG.748</t>
+          <t>HBM945.FSHR.864</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM573.TTLG.748</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM945.FSHR.864</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>HBM575.THQM.284</t>
+          <t>HBM953.KMTG.758</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2115,37 +2077,37 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM575.THQM.284</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM953.KMTG.758</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>HBM575.THQM.284</t>
+          <t>HBM964.FPNH.767</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM575.THQM.284</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM964.FPNH.767</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>HBM622.STKS.394</t>
+          <t>HBM974.CNWK.327</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2161,37 +2123,37 @@
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM622.STKS.394</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM974.CNWK.327</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>HBM622.STKS.394</t>
+          <t>HBM988.SNDW.698</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>preparation_instrument_vendor</t>
+          <t>preparation_instrument_model</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Akoya Biosciences</t>
+          <t>prototype robot - Stanford/Nolan Lab</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM622.STKS.394</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM988.SNDW.698</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>HBM626.VJMB.795</t>
+          <t>HBM996.MDQH.988</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2201,1565 +2163,21 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
+          <t>CODEX Instrument</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM626.VJMB.795</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>HBM626.VJMB.795</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM626.VJMB.795</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>HBM627.KDHD.293</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM627.KDHD.293</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>HBM627.KDHD.293</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM627.KDHD.293</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>HBM666.NDQZ.365</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM666.NDQZ.365</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>HBM666.NDQZ.365</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM666.NDQZ.365</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>HBM666.RBCG.529</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM666.RBCG.529</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>HBM666.RBCG.529</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM666.RBCG.529</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>HBM676.QVGZ.455</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM676.QVGZ.455</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>HBM676.QVGZ.455</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM676.QVGZ.455</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>HBM679.NNNK.283</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM679.NNNK.283</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>HBM679.NNNK.283</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM679.NNNK.283</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>HBM683.NRPR.962</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM683.NRPR.962</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>HBM683.NRPR.962</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM683.NRPR.962</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>HBM687.SJLD.889</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>CODEX Instrument</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM687.SJLD.889</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>HBM687.SJLD.889</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM687.SJLD.889</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>HBM727.DMKG.675</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM727.DMKG.675</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>HBM727.DMKG.675</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM727.DMKG.675</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>HBM729.XTBN.693</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>CODEX Instrument</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM729.XTBN.693</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>HBM729.XTBN.693</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM729.XTBN.693</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>HBM734.XBSR.357</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM734.XBSR.357</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>HBM734.XBSR.357</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM734.XBSR.357</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>HBM739.HCWP.359</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>CODEX Instrument</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM739.HCWP.359</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>HBM739.HCWP.359</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM739.HCWP.359</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>HBM742.NHHQ.357</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM742.NHHQ.357</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>HBM742.NHHQ.357</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM742.NHHQ.357</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>HBM749.SMWP.555</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM749.SMWP.555</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>HBM749.SMWP.555</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM749.SMWP.555</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>HBM772.TKCN.287</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM772.TKCN.287</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>HBM772.TKCN.287</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM772.TKCN.287</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>HBM785.FJVT.469</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM785.FJVT.469</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>HBM785.FJVT.469</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM785.FJVT.469</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>HBM792.FFJT.499</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM792.FFJT.499</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>HBM792.FFJT.499</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM792.FFJT.499</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>HBM823.RJNG.364</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM823.RJNG.364</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>HBM823.RJNG.364</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM823.RJNG.364</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>HBM824.XGWZ.857</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM824.XGWZ.857</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>HBM824.XGWZ.857</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM824.XGWZ.857</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>HBM827.SJBP.777</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM827.SJBP.777</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>HBM827.SJBP.777</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM827.SJBP.777</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>HBM832.ZSQJ.442</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM832.ZSQJ.442</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>HBM832.ZSQJ.442</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM832.ZSQJ.442</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>HBM845.VMSZ.536</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM845.VMSZ.536</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>HBM845.VMSZ.536</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM845.VMSZ.536</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>HBM852.NKST.623</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM852.NKST.623</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>HBM852.NKST.623</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM852.NKST.623</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>HBM865.VDXC.862</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM865.VDXC.862</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>HBM865.VDXC.862</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM865.VDXC.862</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>HBM893.MCGS.487</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>CODEX Instrument</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM893.MCGS.487</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>HBM893.MCGS.487</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM893.MCGS.487</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>HBM899.KTQM.246</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM899.KTQM.246</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>HBM899.KTQM.246</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr"/>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM899.KTQM.246</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>HBM934.KLGL.584</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr"/>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM934.KLGL.584</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>HBM934.KLGL.584</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM934.KLGL.584</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>HBM938.KMNW.825</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM938.KMNW.825</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>HBM938.KMNW.825</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr"/>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM938.KMNW.825</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>HBM945.FSHR.864</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM945.FSHR.864</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>HBM945.FSHR.864</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM945.FSHR.864</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>HBM953.KMTG.758</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM953.KMTG.758</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>HBM953.KMTG.758</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM953.KMTG.758</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>HBM964.FPNH.767</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>CODEX Instrument</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr"/>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM964.FPNH.767</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>HBM964.FPNH.767</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr"/>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM964.FPNH.767</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>HBM974.CNWK.327</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr"/>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM974.CNWK.327</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>HBM974.CNWK.327</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr"/>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM974.CNWK.327</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>HBM988.SNDW.698</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>prototype robot - Stanford/Nolan Lab</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr"/>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM988.SNDW.698</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>HBM988.SNDW.698</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr"/>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM988.SNDW.698</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>HBM996.MDQH.988</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>preparation_instrument_model</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>CODEX Instrument</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="inlineStr">
-        <is>
           <t>https://portal.hubmapconsortium.org/browse/HBM996.MDQH.988</t>
         </is>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>HBM996.MDQH.988</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>preparation_instrument_vendor</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Akoya Biosciences</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr"/>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM996.MDQH.988</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E135"/>
-  <dataValidations count="2">
-    <dataValidation sqref="D2 D4 D6 D8 D10 D12 D14 D16 D18 D20 D22 D24 D26 D28 D30 D32 D34 D36 D38 D40 D42 D44 D46 D48 D50 D52 D54 D56 D58 D60 D62 D64 D66 D68 D70 D72 D74 D76 D78 D80 D82 D84 D86 D88 D90 D92 D94 D96 D98 D100 D102 D104 D106 D108 D110 D112 D114 D116 D118 D120 D122 D124 D126 D128 D130 D132 D134" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$A$1:$A$18</formula1>
-    </dataValidation>
-    <dataValidation sqref="D3 D5 D7 D9 D11 D13 D15 D17 D19 D21 D23 D25 D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D49 D51 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77 D79 D81 D83 D85 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109 D111 D113 D115 D117 D119 D121 D123 D125 D127 D129 D131 D133 D135" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$B$1:$B$9</formula1>
+  <autoFilter ref="A1:E68"/>
+  <dataValidations count="1">
+    <dataValidation sqref="D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
+      <formula1>_validation_data!$A$1:$A$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7496,7 +5914,7 @@
   <autoFilter ref="A1:D206"/>
   <dataValidations count="1">
     <dataValidation sqref="C3 C6 C9 C12 C15 C18 C21 C24 C27 C30 C33 C36 C39 C42 C45 C48 C53 C56 C59 C62 C65 C68 C71 C74 C77 C80 C83 C86 C89 C92 C95 C98 C101 C104 C107 C110 C113 C116 C119 C122 C125 C128 C131 C134 C137 C140 C143 C146 C149 C152 C155 C158 C161 C164 C167 C170 C173 C176 C179 C182 C185 C188 C191 C194 C197 C202 C205" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$C$1:$C$5</formula1>
+      <formula1>_validation_data!$B$1:$B$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>